<commit_message>
add product import file
</commit_message>
<xml_diff>
--- a/public/uploads/product-import.xlsx
+++ b/public/uploads/product-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saim\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\hd-v2\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -135,12 +135,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,8 +161,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +447,7 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,67 +464,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix status on sample sheet
</commit_message>
<xml_diff>
--- a/public/uploads/product-import.xlsx
+++ b/public/uploads/product-import.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\hd-v2\public\uploads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -95,9 +90,6 @@
     <t>test123</t>
   </si>
   <si>
-    <t>active</t>
-  </si>
-  <si>
     <t>mobile</t>
   </si>
   <si>
@@ -110,9 +102,6 @@
     <t>Miami</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>watch</t>
   </si>
   <si>
@@ -120,12 +109,18 @@
   </si>
   <si>
     <t>123A</t>
+  </si>
+  <si>
+    <t>approved</t>
+  </si>
+  <si>
+    <t>pending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -259,7 +254,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -436,7 +431,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,7 +442,7 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,19 +534,19 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>12312</v>
       </c>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2">
         <v>123132</v>
@@ -584,13 +579,13 @@
         <v>500</v>
       </c>
       <c r="S2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T2">
         <v>5</v>
       </c>
       <c r="U2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -603,17 +598,20 @@
       <c r="C3" t="s">
         <v>22</v>
       </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
       <c r="E3">
         <v>12312</v>
       </c>
       <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3">
         <v>123132</v>
@@ -640,13 +638,13 @@
         <v>500</v>
       </c>
       <c r="S3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T3">
         <v>5</v>
       </c>
       <c r="U3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -660,22 +658,22 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>12312312</v>
       </c>
       <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
         <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" t="s">
-        <v>31</v>
       </c>
       <c r="J4" t="s">
         <v>21</v>
@@ -705,13 +703,13 @@
         <v>500</v>
       </c>
       <c r="S4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T4">
         <v>5</v>
       </c>
       <c r="U4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds product policies and fix shcode for product
</commit_message>
<xml_diff>
--- a/public/uploads/product-import.xlsx
+++ b/public/uploads/product-import.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\hd-v2\public\uploads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -123,12 +118,15 @@
   </si>
   <si>
     <t>sku14</t>
+  </si>
+  <si>
+    <t>SH Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -227,7 +225,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -262,7 +260,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -439,7 +437,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +463,7 @@
     <col min="20" max="20" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,8 +524,11 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -588,8 +589,11 @@
       <c r="T2" t="s">
         <v>24</v>
       </c>
+      <c r="U2">
+        <v>210610</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -647,8 +651,11 @@
       <c r="T3" t="s">
         <v>24</v>
       </c>
+      <c r="U3">
+        <v>210610</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -708,6 +715,9 @@
       </c>
       <c r="T4" t="s">
         <v>24</v>
+      </c>
+      <c r="U4">
+        <v>210610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds weight field to sample file
</commit_message>
<xml_diff>
--- a/public/uploads/product-import.xlsx
+++ b/public/uploads/product-import.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>SH Code</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Measurement Unit</t>
+  </si>
+  <si>
+    <t>kg/cm</t>
+  </si>
+  <si>
+    <t>lbs/in</t>
   </si>
 </sst>
 </file>
@@ -445,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,9 +473,10 @@
     <col min="17" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.5703125" customWidth="1"/>
+    <col min="23" max="23" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,8 +540,14 @@
       <c r="U1" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -592,8 +611,14 @@
       <c r="U2">
         <v>210610</v>
       </c>
+      <c r="V2">
+        <v>5</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -654,8 +679,14 @@
       <c r="U3">
         <v>210610</v>
       </c>
+      <c r="V3">
+        <v>6</v>
+      </c>
+      <c r="W3" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -718,6 +749,12 @@
       </c>
       <c r="U4">
         <v>210610</v>
+      </c>
+      <c r="V4">
+        <v>7</v>
+      </c>
+      <c r="W4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>